<commit_message>
Sonar: Put single-quotes around '\"' to use the faster "indexOf(char)" method
</commit_message>
<xml_diff>
--- a/src/test/resources/data/out/playToLogoGame.xlsx
+++ b/src/test/resources/data/out/playToLogoGame.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="32">
   <si>
     <t>Résultat</t>
   </si>
@@ -101,6 +101,18 @@
   </si>
   <si>
     <t>Échec : Brand « heineken » is prohibited.</t>
+  </si>
+  <si>
+    <t>8 / 12</t>
+  </si>
+  <si>
+    <t>12 / 12</t>
+  </si>
+  <si>
+    <t>Alerte : Brand « fake » does not exist.</t>
+  </si>
+  <si>
+    <t>2 / 12</t>
   </si>
 </sst>
 </file>
@@ -108,7 +120,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,6 +166,21 @@
       <sz val="11"/>
       <color indexed="17"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="53"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -254,7 +281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -280,6 +307,9 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -678,9 +708,11 @@
       <c r="B2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="23" t="s">
-        <v>24</v>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>23</v>
       </c>
       <c r="E2" s="3"/>
     </row>
@@ -692,8 +724,8 @@
         <v>16</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="24" t="s">
-        <v>25</v>
+      <c r="D3" s="25" t="s">
+        <v>23</v>
       </c>
       <c r="E3" s="3"/>
     </row>
@@ -705,8 +737,8 @@
         <v>19</v>
       </c>
       <c r="C4" s="6"/>
-      <c r="D4" s="24" t="s">
-        <v>25</v>
+      <c r="D4" s="25" t="s">
+        <v>23</v>
       </c>
       <c r="E4" s="4"/>
     </row>
@@ -718,8 +750,8 @@
         <v>6</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="24" t="s">
-        <v>25</v>
+      <c r="D5" s="25" t="s">
+        <v>23</v>
       </c>
       <c r="E5" s="3"/>
     </row>
@@ -731,8 +763,8 @@
         <v>17</v>
       </c>
       <c r="C6" s="6"/>
-      <c r="D6" s="24" t="s">
-        <v>25</v>
+      <c r="D6" s="25" t="s">
+        <v>23</v>
       </c>
       <c r="E6" s="3"/>
     </row>
@@ -744,8 +776,8 @@
         <v>7</v>
       </c>
       <c r="C7" s="6"/>
-      <c r="D7" s="24" t="s">
-        <v>25</v>
+      <c r="D7" s="25" t="s">
+        <v>23</v>
       </c>
       <c r="E7" s="4"/>
     </row>
@@ -756,9 +788,11 @@
       <c r="B8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="23" t="s">
-        <v>24</v>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>23</v>
       </c>
       <c r="E8" s="3"/>
     </row>
@@ -770,8 +804,8 @@
         <v>16</v>
       </c>
       <c r="C9" s="1"/>
-      <c r="D9" s="24" t="s">
-        <v>25</v>
+      <c r="D9" s="25" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -782,8 +816,8 @@
         <v>8</v>
       </c>
       <c r="C10" s="6"/>
-      <c r="D10" s="24" t="s">
-        <v>25</v>
+      <c r="D10" s="25" t="s">
+        <v>23</v>
       </c>
       <c r="E10" s="3"/>
     </row>
@@ -795,8 +829,8 @@
         <v>9</v>
       </c>
       <c r="C11" s="6"/>
-      <c r="D11" s="24" t="s">
-        <v>25</v>
+      <c r="D11" s="25" t="s">
+        <v>23</v>
       </c>
       <c r="E11" s="3"/>
     </row>
@@ -808,8 +842,8 @@
         <v>19</v>
       </c>
       <c r="C12" s="6"/>
-      <c r="D12" s="24" t="s">
-        <v>25</v>
+      <c r="D12" s="25" t="s">
+        <v>23</v>
       </c>
       <c r="E12" s="4"/>
     </row>
@@ -821,8 +855,8 @@
         <v>6</v>
       </c>
       <c r="C13" s="1"/>
-      <c r="D13" s="24" t="s">
-        <v>25</v>
+      <c r="D13" s="25" t="s">
+        <v>23</v>
       </c>
       <c r="E13" s="3"/>
     </row>
@@ -834,8 +868,8 @@
         <v>17</v>
       </c>
       <c r="C14" s="6"/>
-      <c r="D14" s="24" t="s">
-        <v>25</v>
+      <c r="D14" s="25" t="s">
+        <v>23</v>
       </c>
       <c r="E14" s="3"/>
     </row>
@@ -847,8 +881,8 @@
         <v>7</v>
       </c>
       <c r="C15" s="6"/>
-      <c r="D15" s="24" t="s">
-        <v>25</v>
+      <c r="D15" s="25" t="s">
+        <v>23</v>
       </c>
       <c r="E15" s="4"/>
     </row>
@@ -860,8 +894,8 @@
         <v>8</v>
       </c>
       <c r="C16" s="6"/>
-      <c r="D16" s="24" t="s">
-        <v>25</v>
+      <c r="D16" s="25" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -871,9 +905,11 @@
       <c r="B17" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="23" t="s">
-        <v>24</v>
+      <c r="C17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -884,8 +920,8 @@
         <v>14</v>
       </c>
       <c r="C18" s="6"/>
-      <c r="D18" s="24" t="s">
-        <v>25</v>
+      <c r="D18" s="27" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -896,8 +932,8 @@
         <v>5</v>
       </c>
       <c r="C19" s="6"/>
-      <c r="D19" s="24" t="s">
-        <v>25</v>
+      <c r="D19" s="25" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -908,8 +944,8 @@
         <v>9</v>
       </c>
       <c r="C20" s="6"/>
-      <c r="D20" s="24" t="s">
-        <v>25</v>
+      <c r="D20" s="25" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -920,8 +956,8 @@
         <v>18</v>
       </c>
       <c r="C21" s="6"/>
-      <c r="D21" s="24" t="s">
-        <v>25</v>
+      <c r="D21" s="25" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -932,8 +968,8 @@
         <v>10</v>
       </c>
       <c r="C22" s="6"/>
-      <c r="D22" s="24" t="s">
-        <v>25</v>
+      <c r="D22" s="25" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -944,8 +980,8 @@
         <v>11</v>
       </c>
       <c r="C23" s="6"/>
-      <c r="D23" s="24" t="s">
-        <v>25</v>
+      <c r="D23" s="25" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -956,8 +992,8 @@
         <v>12</v>
       </c>
       <c r="C24" s="6"/>
-      <c r="D24" s="24" t="s">
-        <v>25</v>
+      <c r="D24" s="25" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -967,7 +1003,7 @@
       <c r="B25" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="24" t="s">
+      <c r="D25" s="27" t="s">
         <v>26</v>
       </c>
     </row>
@@ -978,7 +1014,7 @@
       <c r="B26" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="24" t="s">
+      <c r="D26" s="27" t="s">
         <v>26</v>
       </c>
     </row>
@@ -990,7 +1026,7 @@
         <v>21</v>
       </c>
       <c r="C27" s="12"/>
-      <c r="D27" s="23" t="s">
+      <c r="D27" s="26" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1001,7 +1037,7 @@
       <c r="B28" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D28" s="24" t="s">
+      <c r="D28" s="27" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>